<commit_message>
Level 1 - weapons starting to be added, attempt for fps arms
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D0D04C-47A2-4F48-ACD8-5F969D73A95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7D8C0-6CCA-4728-AFB4-687CD818403A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Asthetics" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -133,13 +134,88 @@
   </si>
   <si>
     <t>Power up icons</t>
+  </si>
+  <si>
+    <t>Game TO DO</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>PowerUp</t>
+  </si>
+  <si>
+    <t>Bullets</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>Running(down)</t>
+  </si>
+  <si>
+    <t>Weapon animation</t>
+  </si>
+  <si>
+    <t>Enemy animation</t>
+  </si>
+  <si>
+    <t>Inside of pyramid</t>
+  </si>
+  <si>
+    <t>Game Logic</t>
+  </si>
+  <si>
+    <t>Implement everything</t>
+  </si>
+  <si>
+    <t>NEW STUFF:</t>
+  </si>
+  <si>
+    <t>Ammo limit + finding ammo</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HAXiX0zWklo</t>
+  </si>
+  <si>
+    <t>https://www.mixamo.com/#/?page=1&amp;type=Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 1 </t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/3d/characters/low-poly-skeleton-162347  https://assetstore.unity.com/packages/3d/characters/humanoids/fantasy/skeleton-pbr-animated-low-poly-30659</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/3d/props/weapons/free-low-poly-fantasy-rpg-weapons-248405</t>
+  </si>
+  <si>
+    <t>In Game yet</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/3d/props/low-poly-powerups-212079</t>
+  </si>
+  <si>
+    <t>Staff complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +223,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +272,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,10 +367,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -272,8 +387,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,7 +730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -910,4 +1037,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC5F5D5-1070-419E-8B2A-E19CDFFF0A1C}">
+  <dimension ref="B1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="92.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="F2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="13"/>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{D42B3CE5-61E4-4513-BFAE-EEA65143F339}"/>
+    <hyperlink ref="F9" r:id="rId2" location="/?page=1&amp;type=Character" xr:uid="{813B62C6-5046-4AC4-A44E-F3570EC1DD4D}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://assetstore.unity.com/packages/3d/characters/low-poly-skeleton-162347" xr:uid="{8EFE0F98-0616-4630-88EB-3E77B007FE68}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{1446F3C7-F711-424D-B3F4-ECDA6B90B937}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{B9845682-AF6B-40E6-BA07-118B895A8561}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Level 1 - Progress
Some weapon and powerup progress
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF7D8C0-6CCA-4728-AFB4-687CD818403A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D0AF3-31D4-4223-B367-20B93174EFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthetics" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>Staff complete</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/3d/props/weapons/free-low-poly-swords-rpg-weapons-198166</t>
+  </si>
+  <si>
+    <t>May be</t>
+  </si>
+  <si>
+    <t>Block Heals with E?</t>
   </si>
 </sst>
 </file>
@@ -371,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -398,6 +407,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1041,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC5F5D5-1070-419E-8B2A-E19CDFFF0A1C}">
-  <dimension ref="B1:G21"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,11 +1065,12 @@
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="92.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>36</v>
       </c>
@@ -1069,15 +1082,18 @@
       <c r="G2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="2:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="15" t="s">
@@ -1087,7 +1103,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="15" t="s">
@@ -1099,8 +1115,11 @@
       <c r="G5" s="21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="15" t="s">
@@ -1109,22 +1128,25 @@
       <c r="F6" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
@@ -1134,28 +1156,28 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
       <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="15" t="s">
@@ -1165,19 +1187,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -1221,6 +1243,7 @@
     <hyperlink ref="F4" r:id="rId3" display="https://assetstore.unity.com/packages/3d/characters/low-poly-skeleton-162347" xr:uid="{8EFE0F98-0616-4630-88EB-3E77B007FE68}"/>
     <hyperlink ref="F5" r:id="rId4" xr:uid="{1446F3C7-F711-424D-B3F4-ECDA6B90B937}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{B9845682-AF6B-40E6-BA07-118B895A8561}"/>
+    <hyperlink ref="L5" r:id="rId6" xr:uid="{EB250C36-D4A8-4E22-A269-E6D148333977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Level 1 - Game Logic
Trying to bake navmeshagent onto floor but not working
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78231311-5330-4865-83A8-C3E0DE04F55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2996E8-7765-4966-B565-19538C2D4CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Fifure out how to animate</t>
+  </si>
+  <si>
+    <t>Why can I not navmeshbake the floor</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1062,7 @@
   <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,39 +1210,42 @@
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
       <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G18" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Level 1 - Preffabing
Fire, light, audio
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2996E8-7765-4966-B565-19538C2D4CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5B34F1-1184-4221-B4E0-73EFC17A9389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1062,7 +1062,7 @@
   <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Level 1 changes + User Testing Doc
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2507F9-7763-49CB-9013-21C98483B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1016CE47-EFDD-4BD7-8B4B-32305BD686D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthetics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>Lighting does not work</t>
+  </si>
+  <si>
+    <t>Enemy clipping and the height</t>
+  </si>
+  <si>
+    <t>Also scaling moves ui</t>
+  </si>
+  <si>
+    <t>Add by tomo</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Enemy working</t>
+  </si>
+  <si>
+    <t>Game end</t>
+  </si>
+  <si>
+    <t>Boss working</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D09A13-966C-4B9A-8C39-B15C391C9D84}">
-  <dimension ref="B4:D5"/>
+  <dimension ref="B4:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,20 +1313,52 @@
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level 1 - Fixed pyramid with navmesh was not baked onto csg model
altho they cant go thro the door now  + blindspots, will need to be fixed tms
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1016CE47-EFDD-4BD7-8B4B-32305BD686D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818F5600-7CDD-45CF-9B24-0801907F3E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Boss working</t>
+  </si>
+  <si>
+    <t>Lots of issues with the navmesh, certain blind spots, the pyramid is not perfect either still cant enter thro door</t>
   </si>
 </sst>
 </file>
@@ -1300,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D09A13-966C-4B9A-8C39-B15C391C9D84}">
-  <dimension ref="B4:G9"/>
+  <dimension ref="B4:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,9 +1314,10 @@
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>66</v>
       </c>
@@ -1323,8 +1327,11 @@
       <c r="G4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J4" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
@@ -1335,12 +1342,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>70</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>71</v>
       </c>
@@ -1356,7 +1363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Level 1 - finalising ui
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818F5600-7CDD-45CF-9B24-0801907F3E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E14B1B-77EE-4940-B498-9FA7D54F8EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthetics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -261,6 +261,24 @@
   </si>
   <si>
     <t>Lots of issues with the navmesh, certain blind spots, the pyramid is not perfect either still cant enter thro door</t>
+  </si>
+  <si>
+    <t>The fucking animation works but it wont trigger because the enemy keeps glitching below and I have no idea why</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have tried so much to fix it </t>
+  </si>
+  <si>
+    <t>I think the issue is navmesh</t>
+  </si>
+  <si>
+    <t>ok the issue is my navmeshagent as i have a model with animation but no navmeshagent and it works, also when i apply a navmeshagaent it resizes the enemy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FONT TO USE </t>
+  </si>
+  <si>
+    <t>GeosansLight</t>
   </si>
 </sst>
 </file>
@@ -284,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +375,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -423,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -454,6 +484,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +869,7 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
@@ -845,7 +877,7 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
@@ -869,23 +901,27 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
@@ -901,7 +937,7 @@
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
@@ -909,7 +945,7 @@
       <c r="D14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
@@ -917,7 +953,7 @@
       <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
@@ -925,17 +961,17 @@
       <c r="D16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -943,7 +979,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -951,7 +987,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2" t="s">
@@ -959,7 +995,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="2" t="s">
@@ -967,7 +1003,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
@@ -975,13 +1011,13 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
         <v>21</v>
@@ -989,7 +1025,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
@@ -997,23 +1033,25 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="2" t="s">
@@ -1021,7 +1059,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1029,7 +1067,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="10" t="s">
@@ -1037,7 +1075,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
@@ -1045,19 +1083,19 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
@@ -1065,29 +1103,32 @@
       <c r="D34" s="5"/>
       <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="25"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="11"/>
+      <c r="F37" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1303,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D09A13-966C-4B9A-8C39-B15C391C9D84}">
-  <dimension ref="B4:J9"/>
+  <dimension ref="B4:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,9 +1356,10 @@
     <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="43.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>66</v>
       </c>
@@ -1331,7 +1373,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>67</v>
       </c>
@@ -1342,12 +1384,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>70</v>
       </c>
@@ -1355,17 +1397,31 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>71</v>
       </c>
       <c r="G8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>76</v>
+      </c>
+      <c r="J9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level 1 - Staff noise + background music
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E14B1B-77EE-4940-B498-9FA7D54F8EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF28D58F-88AE-4C20-B8D0-94256A4B2B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>GeosansLight</t>
+  </si>
+  <si>
+    <t>BACKGROUND MUSIC ADDED</t>
+  </si>
+  <si>
+    <t>For the staff yeh</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -486,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -818,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +970,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="8" t="s">
@@ -971,7 +978,7 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -979,7 +986,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -987,7 +994,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2" t="s">
@@ -995,7 +1002,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="2" t="s">
@@ -1003,7 +1010,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
@@ -1011,13 +1018,13 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
         <v>21</v>
@@ -1025,7 +1032,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
@@ -1033,25 +1040,31 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="12"/>
+      <c r="F27" s="26"/>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="2" t="s">
@@ -1059,7 +1072,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1067,7 +1080,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="10" t="s">
@@ -1075,7 +1088,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
@@ -1083,7 +1096,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>

</xml_diff>

<commit_message>
Level 1 - wavemanager refined
now there are no issues with wavemanager
</commit_message>
<xml_diff>
--- a/Documentation/Tracker.xlsx
+++ b/Documentation/Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\3000\Timeline-Takedown\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF28D58F-88AE-4C20-B8D0-94256A4B2B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38217B3B-CDA8-4630-B2F7-C13CEEB8C3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthetics" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>OBJECTIVE</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Game Logic</t>
   </si>
   <si>
-    <t>Implement everything</t>
-  </si>
-  <si>
     <t>NEW STUFF:</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
     <t>Lots of issues with the navmesh, certain blind spots, the pyramid is not perfect either still cant enter thro door</t>
   </si>
   <si>
-    <t>The fucking animation works but it wont trigger because the enemy keeps glitching below and I have no idea why</t>
-  </si>
-  <si>
     <t xml:space="preserve">I have tried so much to fix it </t>
   </si>
   <si>
@@ -285,6 +279,21 @@
   </si>
   <si>
     <t>For the staff yeh</t>
+  </si>
+  <si>
+    <t>The animation works but it wont trigger because the enemy keeps glitching below and I have no idea why</t>
+  </si>
+  <si>
+    <t>Audio or visual que when wave goes to next (in the 5sec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boss drop </t>
+  </si>
+  <si>
+    <t>Timer between rounds, fix the issue of enemys left over from round</t>
+  </si>
+  <si>
+    <t>Enemy health also had to be changed as it was calling multiple death calls for some reason but now there is a isdead flag to make sure the enemy can only die once</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -492,7 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -823,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G37"/>
+  <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +844,7 @@
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -912,7 +921,7 @@
     </row>
     <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2" t="s">
@@ -922,7 +931,7 @@
     </row>
     <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
@@ -970,7 +979,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="8" t="s">
@@ -978,7 +987,7 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -986,7 +995,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -994,15 +1003,18 @@
       <c r="D19" s="5"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="2" t="s">
@@ -1010,7 +1022,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
@@ -1018,13 +1030,13 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
         <v>21</v>
@@ -1032,7 +1044,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="2" t="s">
@@ -1040,7 +1052,7 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="2" t="s">
@@ -1049,22 +1061,21 @@
       <c r="E26" s="12"/>
       <c r="F26" s="25"/>
       <c r="G26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="12"/>
-      <c r="F27" s="26"/>
       <c r="G27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="2" t="s">
@@ -1072,7 +1083,7 @@
       </c>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1080,7 +1091,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="10" t="s">
@@ -1088,7 +1099,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
@@ -1096,7 +1107,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1154,7 +1165,7 @@
   <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,13 +1186,13 @@
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="F2" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1198,7 +1209,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1208,13 +1219,13 @@
         <v>39</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1224,10 +1235,10 @@
         <v>40</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1248,10 +1259,10 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1282,7 +1293,7 @@
         <v>45</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1313,24 +1324,24 @@
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="15" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1339,7 +1350,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1357,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D09A13-966C-4B9A-8C39-B15C391C9D84}">
-  <dimension ref="B4:K10"/>
+  <dimension ref="B4:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,27 +1385,27 @@
   <sheetData>
     <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -1404,37 +1415,47 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>